<commit_message>
more log - videos, max_saved_data
</commit_message>
<xml_diff>
--- a/experiments/20-01-22_12-41-12_stiffness-only.xlsx
+++ b/experiments/20-01-22_12-41-12_stiffness-only.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yijiangh\Documents\pb_ws\pb-construction\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE689F72-D0B0-4C7C-BDF5-3124F450199E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50899A9D-63BE-469F-A49F-D5AF32ECE215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="109">
   <si>
     <t>config_id</t>
   </si>
@@ -1127,6 +1127,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="409090320"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3176,7 +3177,7 @@
   <dimension ref="A1:U493"/>
   <sheetViews>
     <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S61" sqref="B51:S61"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23263,8 +23264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180455DA-5CB5-4AA5-9712-CD7D27B0A0B7}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23284,6 +23285,10 @@
       <c r="C1" t="s">
         <v>36</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C2" t="s">

</xml_diff>